<commit_message>
Actualizar XLSX con datos del día
</commit_message>
<xml_diff>
--- a/public/operaciones.xlsx
+++ b/public/operaciones.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\saulm\Desktop\PAGINA ATFM\ATFM-dashboard_v1.2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\saulm\Desktop\PAGINA ATFM\ATFM-dashboard-taf\taf-site\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17EC5AF4-E7F1-4783-9489-03799F60B299}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F0A2870-D258-4928-8D11-5CF9A9AA8E6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{4661D124-5B3F-4151-B830-E4D5C481018A}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="48">
   <si>
     <t>AEROLINEA</t>
   </si>
@@ -125,9 +125,6 @@
     <t>KDFW</t>
   </si>
   <si>
-    <t>KBOS</t>
-  </si>
-  <si>
     <t>CYYZ</t>
   </si>
   <si>
@@ -161,19 +158,28 @@
     <t>AJT</t>
   </si>
   <si>
-    <t>TPA</t>
-  </si>
-  <si>
-    <t>TAG</t>
-  </si>
-  <si>
-    <t>MHRO</t>
-  </si>
-  <si>
     <t>NKS</t>
   </si>
   <si>
     <t>KFLL</t>
+  </si>
+  <si>
+    <t>SEGU</t>
+  </si>
+  <si>
+    <t>KONT</t>
+  </si>
+  <si>
+    <t>MMUN</t>
+  </si>
+  <si>
+    <t>FDX</t>
+  </si>
+  <si>
+    <t>VOC</t>
+  </si>
+  <si>
+    <t>MHTG</t>
   </si>
 </sst>
 </file>
@@ -579,8 +585,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5321A0FC-476F-46FE-A6F3-676ADAB60D1D}">
   <dimension ref="A1:G140"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A133" workbookViewId="0">
-      <selection activeCell="A150" sqref="A150"/>
+    <sheetView tabSelected="1" topLeftCell="A121" workbookViewId="0">
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -628,91 +634,91 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="B3" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="C3" s="1">
-        <v>0.20138888888888887</v>
+        <v>0.15972222222222224</v>
       </c>
       <c r="D3">
-        <v>1266</v>
+        <v>222</v>
       </c>
       <c r="G3" s="1"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B4" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C4" s="1">
-        <v>0.20624999999999999</v>
+        <v>0.20138888888888887</v>
       </c>
       <c r="D4">
-        <v>4313</v>
+        <v>1266</v>
       </c>
       <c r="G4" s="1"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B5" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C5" s="1">
-        <v>0.20833333333333334</v>
+        <v>0.20624999999999999</v>
       </c>
       <c r="D5">
-        <v>456</v>
+        <v>4313</v>
       </c>
       <c r="G5" s="1"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="C6" s="1"/>
       <c r="E6">
-        <v>879</v>
+        <v>224</v>
       </c>
       <c r="F6" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="G6" s="1">
-        <v>0.21111111111111111</v>
+        <v>0.20833333333333334</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>11</v>
-      </c>
-      <c r="B7" t="s">
-        <v>16</v>
-      </c>
-      <c r="C7" s="1">
-        <v>0.21180555555555555</v>
-      </c>
-      <c r="D7">
-        <v>428</v>
-      </c>
-      <c r="G7" s="1"/>
+        <v>14</v>
+      </c>
+      <c r="C7" s="1"/>
+      <c r="E7">
+        <v>879</v>
+      </c>
+      <c r="F7" t="s">
+        <v>15</v>
+      </c>
+      <c r="G7" s="1">
+        <v>0.21111111111111111</v>
+      </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>11</v>
       </c>
       <c r="B8" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C8" s="1">
-        <v>0.22222222222222221</v>
+        <v>0.21180555555555555</v>
       </c>
       <c r="D8">
-        <v>575</v>
+        <v>428</v>
       </c>
       <c r="G8" s="1"/>
     </row>
@@ -720,134 +726,134 @@
       <c r="A9" t="s">
         <v>11</v>
       </c>
-      <c r="C9" s="1"/>
-      <c r="E9">
-        <v>556</v>
-      </c>
-      <c r="F9" t="s">
-        <v>23</v>
-      </c>
-      <c r="G9" s="1">
-        <v>0.22916666666666666</v>
-      </c>
+      <c r="B9" t="s">
+        <v>42</v>
+      </c>
+      <c r="C9" s="1">
+        <v>0.21180555555555555</v>
+      </c>
+      <c r="D9">
+        <v>592</v>
+      </c>
+      <c r="G9" s="1"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>9</v>
-      </c>
-      <c r="C10" s="1"/>
-      <c r="E10">
-        <v>4350</v>
-      </c>
-      <c r="F10" t="s">
-        <v>19</v>
-      </c>
-      <c r="G10" s="1">
-        <v>0.22916666666666666</v>
-      </c>
+        <v>11</v>
+      </c>
+      <c r="B10" t="s">
+        <v>43</v>
+      </c>
+      <c r="C10" s="1">
+        <v>0.21180555555555555</v>
+      </c>
+      <c r="D10">
+        <v>531</v>
+      </c>
+      <c r="G10" s="1"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>11</v>
       </c>
       <c r="B11" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C11" s="1">
-        <v>0.2326388888888889</v>
+        <v>0.22222222222222221</v>
       </c>
       <c r="D11">
-        <v>453</v>
+        <v>575</v>
       </c>
       <c r="G11" s="1"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>9</v>
-      </c>
-      <c r="B12" t="s">
-        <v>8</v>
-      </c>
-      <c r="C12" s="1">
-        <v>0.23472222222222222</v>
-      </c>
-      <c r="D12">
-        <v>4309</v>
-      </c>
-      <c r="G12" s="1"/>
+        <v>11</v>
+      </c>
+      <c r="C12" s="1"/>
+      <c r="E12">
+        <v>556</v>
+      </c>
+      <c r="F12" t="s">
+        <v>23</v>
+      </c>
+      <c r="G12" s="1">
+        <v>0.22916666666666666</v>
+      </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>11</v>
-      </c>
-      <c r="B13" t="s">
-        <v>8</v>
-      </c>
-      <c r="C13" s="1">
-        <v>0.24305555555555555</v>
-      </c>
-      <c r="D13">
-        <v>521</v>
-      </c>
-      <c r="G13" s="1"/>
+        <v>9</v>
+      </c>
+      <c r="C13" s="1"/>
+      <c r="E13">
+        <v>4350</v>
+      </c>
+      <c r="F13" t="s">
+        <v>19</v>
+      </c>
+      <c r="G13" s="1">
+        <v>0.22916666666666666</v>
+      </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>11</v>
       </c>
       <c r="B14" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="C14" s="1">
-        <v>0.24652777777777779</v>
+        <v>0.2326388888888889</v>
       </c>
       <c r="D14">
-        <v>567</v>
+        <v>453</v>
       </c>
       <c r="G14" s="1"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B15" t="s">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="C15" s="1">
-        <v>0.25</v>
+        <v>0.23472222222222222</v>
       </c>
       <c r="D15">
-        <v>366</v>
+        <v>4309</v>
       </c>
       <c r="G15" s="1"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>7</v>
-      </c>
-      <c r="C16" s="1"/>
-      <c r="E16">
-        <v>1467</v>
-      </c>
-      <c r="F16" t="s">
-        <v>22</v>
-      </c>
-      <c r="G16" s="1">
-        <v>0.25</v>
-      </c>
+        <v>11</v>
+      </c>
+      <c r="B16" t="s">
+        <v>8</v>
+      </c>
+      <c r="C16" s="1">
+        <v>0.24305555555555555</v>
+      </c>
+      <c r="D16">
+        <v>521</v>
+      </c>
+      <c r="G16" s="1"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>11</v>
       </c>
       <c r="B17" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="C17" s="1">
-        <v>0.25694444444444442</v>
+        <v>0.24652777777777779</v>
       </c>
       <c r="D17">
-        <v>579</v>
+        <v>567</v>
       </c>
       <c r="G17" s="1"/>
     </row>
@@ -856,29 +862,29 @@
         <v>11</v>
       </c>
       <c r="B18" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C18" s="1">
-        <v>0.2638888888888889</v>
+        <v>0.25</v>
       </c>
       <c r="D18">
-        <v>314</v>
+        <v>366</v>
       </c>
       <c r="G18" s="1"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C19" s="1"/>
       <c r="E19">
-        <v>4326</v>
+        <v>1467</v>
       </c>
       <c r="F19" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="G19" s="1">
-        <v>0.2638888888888889</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
@@ -886,13 +892,13 @@
         <v>11</v>
       </c>
       <c r="B20" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="C20" s="1">
-        <v>0.2673611111111111</v>
+        <v>0.25694444444444442</v>
       </c>
       <c r="D20">
-        <v>650</v>
+        <v>579</v>
       </c>
       <c r="G20" s="1"/>
     </row>
@@ -901,13 +907,13 @@
         <v>11</v>
       </c>
       <c r="B21" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="C21" s="1">
-        <v>0.2673611111111111</v>
+        <v>0.2638888888888889</v>
       </c>
       <c r="D21">
-        <v>626</v>
+        <v>314</v>
       </c>
       <c r="G21" s="1"/>
     </row>
@@ -931,13 +937,13 @@
         <v>11</v>
       </c>
       <c r="B23" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="C23" s="1">
-        <v>0.27083333333333331</v>
+        <v>0.2673611111111111</v>
       </c>
       <c r="D23">
-        <v>561</v>
+        <v>650</v>
       </c>
       <c r="G23" s="1"/>
     </row>
@@ -946,13 +952,13 @@
         <v>11</v>
       </c>
       <c r="B24" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C24" s="1">
         <v>0.27083333333333331</v>
       </c>
       <c r="D24">
-        <v>571</v>
+        <v>561</v>
       </c>
       <c r="G24" s="1"/>
     </row>
@@ -961,13 +967,13 @@
         <v>11</v>
       </c>
       <c r="B25" t="s">
-        <v>10</v>
+        <v>26</v>
       </c>
       <c r="C25" s="1">
         <v>0.27083333333333331</v>
       </c>
       <c r="D25">
-        <v>591</v>
+        <v>571</v>
       </c>
       <c r="G25" s="1"/>
     </row>
@@ -982,24 +988,24 @@
         <v>0.27083333333333331</v>
       </c>
       <c r="D26">
-        <v>691</v>
+        <v>591</v>
       </c>
       <c r="G26" s="1"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>41</v>
-      </c>
-      <c r="B27" t="s">
+        <v>9</v>
+      </c>
+      <c r="C27" s="1"/>
+      <c r="E27">
+        <v>4338</v>
+      </c>
+      <c r="F27" t="s">
         <v>27</v>
       </c>
-      <c r="C27" s="1">
-        <v>0.27083333333333331</v>
-      </c>
-      <c r="D27">
-        <v>4257</v>
-      </c>
-      <c r="G27" s="1"/>
+      <c r="G27" s="1">
+        <v>0.27777777777777779</v>
+      </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
@@ -1007,59 +1013,59 @@
       </c>
       <c r="C28" s="1"/>
       <c r="E28">
-        <v>4338</v>
+        <v>4316</v>
       </c>
       <c r="F28" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="G28" s="1">
-        <v>0.27777777777777779</v>
+        <v>0.28611111111111109</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="B29" t="s">
-        <v>23</v>
+        <v>8</v>
       </c>
       <c r="C29" s="1">
-        <v>0.28125</v>
+        <v>0.29166666666666669</v>
       </c>
       <c r="D29">
-        <v>931</v>
+        <v>529</v>
       </c>
       <c r="G29" s="1"/>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C30" s="1"/>
       <c r="E30">
-        <v>4316</v>
+        <v>323</v>
       </c>
       <c r="F30" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="G30" s="1">
-        <v>0.28611111111111109</v>
+        <v>0.3125</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>11</v>
       </c>
-      <c r="B31" t="s">
-        <v>8</v>
-      </c>
-      <c r="C31" s="1">
-        <v>0.29166666666666669</v>
-      </c>
-      <c r="D31">
-        <v>529</v>
-      </c>
-      <c r="G31" s="1"/>
+      <c r="C31" s="1"/>
+      <c r="E31">
+        <v>396</v>
+      </c>
+      <c r="F31" t="s">
+        <v>24</v>
+      </c>
+      <c r="G31" s="1">
+        <v>0.3125</v>
+      </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
@@ -1067,10 +1073,10 @@
       </c>
       <c r="C32" s="1"/>
       <c r="E32">
-        <v>323</v>
+        <v>562</v>
       </c>
       <c r="F32" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="G32" s="1">
         <v>0.3125</v>
@@ -1082,10 +1088,10 @@
       </c>
       <c r="C33" s="1"/>
       <c r="E33">
-        <v>396</v>
+        <v>639</v>
       </c>
       <c r="F33" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="G33" s="1">
         <v>0.3125</v>
@@ -1097,13 +1103,13 @@
       </c>
       <c r="C34" s="1"/>
       <c r="E34">
-        <v>562</v>
+        <v>310</v>
       </c>
       <c r="F34" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="G34" s="1">
-        <v>0.3125</v>
+        <v>0.31597222222222221</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
@@ -1112,44 +1118,44 @@
       </c>
       <c r="C35" s="1"/>
       <c r="E35">
-        <v>639</v>
+        <v>440</v>
       </c>
       <c r="F35" t="s">
-        <v>19</v>
+        <v>28</v>
       </c>
       <c r="G35" s="1">
-        <v>0.3125</v>
+        <v>0.31944444444444442</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="C36" s="1"/>
       <c r="E36">
-        <v>932</v>
+        <v>536</v>
       </c>
       <c r="F36" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="G36" s="1">
-        <v>0.3125</v>
+        <v>0.31944444444444442</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>11</v>
       </c>
-      <c r="C37" s="1"/>
-      <c r="E37">
-        <v>310</v>
-      </c>
-      <c r="F37" t="s">
-        <v>27</v>
-      </c>
-      <c r="G37" s="1">
-        <v>0.31597222222222221</v>
-      </c>
+      <c r="B37" t="s">
+        <v>10</v>
+      </c>
+      <c r="C37" s="1">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="D37">
+        <v>581</v>
+      </c>
+      <c r="G37" s="1"/>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
@@ -1157,13 +1163,13 @@
       </c>
       <c r="C38" s="1"/>
       <c r="E38">
-        <v>440</v>
+        <v>368</v>
       </c>
       <c r="F38" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="G38" s="1">
-        <v>0.31944444444444442</v>
+        <v>0.33333333333333331</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
@@ -1172,58 +1178,58 @@
       </c>
       <c r="C39" s="1"/>
       <c r="E39">
-        <v>444</v>
+        <v>522</v>
       </c>
       <c r="F39" t="s">
-        <v>29</v>
+        <v>8</v>
       </c>
       <c r="G39" s="1">
-        <v>0.32291666666666669</v>
+        <v>0.33333333333333331</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>11</v>
       </c>
-      <c r="B40" t="s">
-        <v>10</v>
-      </c>
-      <c r="C40" s="1">
-        <v>0.33333333333333331</v>
-      </c>
-      <c r="D40">
-        <v>581</v>
-      </c>
-      <c r="G40" s="1"/>
+      <c r="C40" s="1"/>
+      <c r="E40">
+        <v>626</v>
+      </c>
+      <c r="F40" t="s">
+        <v>29</v>
+      </c>
+      <c r="G40" s="1">
+        <v>0.34027777777777773</v>
+      </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>14</v>
-      </c>
-      <c r="B41" t="s">
-        <v>15</v>
-      </c>
-      <c r="C41" s="1">
-        <v>0.33333333333333331</v>
-      </c>
-      <c r="D41">
-        <v>8918</v>
-      </c>
-      <c r="G41" s="1"/>
+        <v>11</v>
+      </c>
+      <c r="C41" s="1"/>
+      <c r="E41">
+        <v>572</v>
+      </c>
+      <c r="F41" t="s">
+        <v>23</v>
+      </c>
+      <c r="G41" s="1">
+        <v>0.34375</v>
+      </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="C42" s="1"/>
       <c r="E42">
-        <v>368</v>
+        <v>884</v>
       </c>
       <c r="F42" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="G42" s="1">
-        <v>0.33333333333333331</v>
+        <v>0.35625000000000001</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
@@ -1232,44 +1238,44 @@
       </c>
       <c r="C43" s="1"/>
       <c r="E43">
-        <v>522</v>
+        <v>430</v>
       </c>
       <c r="F43" t="s">
-        <v>8</v>
+        <v>30</v>
       </c>
       <c r="G43" s="1">
-        <v>0.33333333333333331</v>
+        <v>0.3611111111111111</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>41</v>
+        <v>11</v>
       </c>
       <c r="C44" s="1"/>
       <c r="E44">
-        <v>4257</v>
+        <v>369</v>
       </c>
       <c r="F44" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G44" s="1">
-        <v>0.33333333333333331</v>
+        <v>0.37847222222222227</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>11</v>
       </c>
-      <c r="C45" s="1"/>
-      <c r="E45">
-        <v>454</v>
-      </c>
-      <c r="F45" t="s">
-        <v>32</v>
-      </c>
-      <c r="G45" s="1">
-        <v>0.33680555555555558</v>
-      </c>
+      <c r="B45" t="s">
+        <v>21</v>
+      </c>
+      <c r="C45" s="1">
+        <v>0.38541666666666669</v>
+      </c>
+      <c r="D45">
+        <v>70</v>
+      </c>
+      <c r="G45" s="1"/>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
@@ -1277,28 +1283,28 @@
       </c>
       <c r="C46" s="1"/>
       <c r="E46">
-        <v>626</v>
+        <v>383</v>
       </c>
       <c r="F46" t="s">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="G46" s="1">
-        <v>0.34027777777777773</v>
+        <v>0.3923611111111111</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C47" s="1"/>
       <c r="E47">
-        <v>554</v>
+        <v>4320</v>
       </c>
       <c r="F47" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G47" s="1">
-        <v>0.34375</v>
+        <v>0.39374999999999999</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
@@ -1307,29 +1313,29 @@
       </c>
       <c r="C48" s="1"/>
       <c r="E48">
-        <v>572</v>
+        <v>582</v>
       </c>
       <c r="F48" t="s">
-        <v>23</v>
+        <v>10</v>
       </c>
       <c r="G48" s="1">
-        <v>0.34375</v>
+        <v>0.39583333333333331</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>14</v>
-      </c>
-      <c r="C49" s="1"/>
-      <c r="E49">
-        <v>884</v>
-      </c>
-      <c r="F49" t="s">
-        <v>15</v>
-      </c>
-      <c r="G49" s="1">
-        <v>0.35625000000000001</v>
-      </c>
+        <v>11</v>
+      </c>
+      <c r="B49" t="s">
+        <v>26</v>
+      </c>
+      <c r="C49" s="1">
+        <v>0.40625</v>
+      </c>
+      <c r="D49">
+        <v>569</v>
+      </c>
+      <c r="G49" s="1"/>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
@@ -1337,43 +1343,43 @@
       </c>
       <c r="C50" s="1"/>
       <c r="E50">
-        <v>430</v>
+        <v>609</v>
       </c>
       <c r="F50" t="s">
-        <v>31</v>
+        <v>19</v>
       </c>
       <c r="G50" s="1">
-        <v>0.3611111111111111</v>
+        <v>0.4201388888888889</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B51" t="s">
         <v>27</v>
       </c>
       <c r="C51" s="1">
-        <v>0.36944444444444446</v>
+        <v>0.42708333333333331</v>
       </c>
       <c r="D51">
-        <v>4257</v>
+        <v>721</v>
       </c>
       <c r="G51" s="1"/>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C52" s="1"/>
       <c r="E52">
-        <v>8918</v>
+        <v>71</v>
       </c>
       <c r="F52" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="G52" s="1">
-        <v>0.375</v>
+        <v>0.42708333333333331</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
@@ -1382,13 +1388,13 @@
       </c>
       <c r="C53" s="1"/>
       <c r="E53">
-        <v>369</v>
+        <v>650</v>
       </c>
       <c r="F53" t="s">
-        <v>12</v>
+        <v>44</v>
       </c>
       <c r="G53" s="1">
-        <v>0.37847222222222227</v>
+        <v>0.43055555555555558</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
@@ -1396,13 +1402,13 @@
         <v>11</v>
       </c>
       <c r="B54" t="s">
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="C54" s="1">
-        <v>0.38541666666666669</v>
+        <v>0.44791666666666669</v>
       </c>
       <c r="D54">
-        <v>70</v>
+        <v>455</v>
       </c>
       <c r="G54" s="1"/>
     </row>
@@ -1410,76 +1416,76 @@
       <c r="A55" t="s">
         <v>11</v>
       </c>
-      <c r="C55" s="1"/>
-      <c r="E55">
-        <v>383</v>
-      </c>
-      <c r="F55" t="s">
-        <v>21</v>
-      </c>
-      <c r="G55" s="1">
-        <v>0.3923611111111111</v>
-      </c>
+      <c r="B55" t="s">
+        <v>23</v>
+      </c>
+      <c r="C55" s="1">
+        <v>0.4513888888888889</v>
+      </c>
+      <c r="D55">
+        <v>573</v>
+      </c>
+      <c r="G55" s="1"/>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>9</v>
-      </c>
-      <c r="C56" s="1"/>
-      <c r="E56">
-        <v>4320</v>
-      </c>
-      <c r="F56" t="s">
-        <v>22</v>
-      </c>
-      <c r="G56" s="1">
-        <v>0.39374999999999999</v>
-      </c>
+        <v>11</v>
+      </c>
+      <c r="B56" t="s">
+        <v>19</v>
+      </c>
+      <c r="C56" s="1">
+        <v>0.4513888888888889</v>
+      </c>
+      <c r="D56">
+        <v>638</v>
+      </c>
+      <c r="G56" s="1"/>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>11</v>
+        <v>39</v>
       </c>
       <c r="C57" s="1"/>
       <c r="E57">
-        <v>582</v>
+        <v>720</v>
       </c>
       <c r="F57" t="s">
-        <v>10</v>
+        <v>27</v>
       </c>
       <c r="G57" s="1">
-        <v>0.39583333333333331</v>
+        <v>0.47916666666666669</v>
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>11</v>
-      </c>
-      <c r="C58" s="1"/>
-      <c r="E58">
-        <v>392</v>
-      </c>
-      <c r="F58" t="s">
-        <v>24</v>
-      </c>
-      <c r="G58" s="1">
-        <v>0.40277777777777779</v>
-      </c>
+        <v>32</v>
+      </c>
+      <c r="B58" t="s">
+        <v>27</v>
+      </c>
+      <c r="C58" s="1">
+        <v>0.4826388888888889</v>
+      </c>
+      <c r="D58">
+        <v>927</v>
+      </c>
+      <c r="G58" s="1"/>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>11</v>
       </c>
-      <c r="B59" t="s">
-        <v>26</v>
-      </c>
-      <c r="C59" s="1">
-        <v>0.40625</v>
-      </c>
-      <c r="D59">
-        <v>569</v>
-      </c>
-      <c r="G59" s="1"/>
+      <c r="C59" s="1"/>
+      <c r="E59">
+        <v>584</v>
+      </c>
+      <c r="F59" t="s">
+        <v>10</v>
+      </c>
+      <c r="G59" s="1">
+        <v>0.49305555555555558</v>
+      </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
@@ -1487,402 +1493,402 @@
       </c>
       <c r="C60" s="1"/>
       <c r="E60">
-        <v>611</v>
+        <v>442</v>
       </c>
       <c r="F60" t="s">
-        <v>19</v>
+        <v>28</v>
       </c>
       <c r="G60" s="1">
-        <v>0.4201388888888889</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>11</v>
-      </c>
-      <c r="C61" s="1"/>
-      <c r="E61">
-        <v>71</v>
-      </c>
-      <c r="F61" t="s">
-        <v>21</v>
-      </c>
-      <c r="G61" s="1">
-        <v>0.42708333333333331</v>
-      </c>
+        <v>7</v>
+      </c>
+      <c r="B61" t="s">
+        <v>22</v>
+      </c>
+      <c r="C61" s="1">
+        <v>0.50416666666666665</v>
+      </c>
+      <c r="D61">
+        <v>1441</v>
+      </c>
+      <c r="G61" s="1"/>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>41</v>
-      </c>
-      <c r="C62" s="1"/>
-      <c r="E62">
-        <v>4257</v>
-      </c>
-      <c r="F62" t="s">
-        <v>13</v>
-      </c>
-      <c r="G62" s="1">
-        <v>0.43194444444444446</v>
-      </c>
+        <v>33</v>
+      </c>
+      <c r="B62" t="s">
+        <v>34</v>
+      </c>
+      <c r="C62" s="1">
+        <v>0.50972222222222219</v>
+      </c>
+      <c r="D62">
+        <v>1910</v>
+      </c>
+      <c r="G62" s="1"/>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>11</v>
       </c>
-      <c r="B63" t="s">
-        <v>32</v>
-      </c>
-      <c r="C63" s="1">
-        <v>0.44791666666666669</v>
-      </c>
-      <c r="D63">
-        <v>455</v>
-      </c>
-      <c r="G63" s="1"/>
+      <c r="C63" s="1"/>
+      <c r="E63">
+        <v>319</v>
+      </c>
+      <c r="F63" t="s">
+        <v>19</v>
+      </c>
+      <c r="G63" s="1">
+        <v>0.51388888888888884</v>
+      </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>40</v>
-      </c>
-      <c r="B64" t="s">
+        <v>32</v>
+      </c>
+      <c r="C64" s="1"/>
+      <c r="E64">
+        <v>1508</v>
+      </c>
+      <c r="F64" t="s">
         <v>27</v>
       </c>
-      <c r="C64" s="1">
-        <v>0.46875</v>
-      </c>
-      <c r="D64">
-        <v>771</v>
-      </c>
-      <c r="G64" s="1"/>
+      <c r="G64" s="1">
+        <v>0.52430555555555558</v>
+      </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>33</v>
+        <v>14</v>
       </c>
       <c r="B65" t="s">
-        <v>27</v>
+        <v>15</v>
       </c>
       <c r="C65" s="1">
-        <v>0.4826388888888889</v>
+        <v>0.52500000000000002</v>
       </c>
       <c r="D65">
-        <v>927</v>
+        <v>816</v>
       </c>
       <c r="G65" s="1"/>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>11</v>
-      </c>
-      <c r="C66" s="1"/>
-      <c r="E66">
-        <v>424</v>
-      </c>
-      <c r="F66" t="s">
-        <v>22</v>
-      </c>
-      <c r="G66" s="1">
-        <v>0.50347222222222221</v>
-      </c>
+        <v>40</v>
+      </c>
+      <c r="B66" t="s">
+        <v>41</v>
+      </c>
+      <c r="C66" s="1">
+        <v>0.52777777777777779</v>
+      </c>
+      <c r="D66">
+        <v>1031</v>
+      </c>
+      <c r="G66" s="1"/>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>7</v>
+        <v>45</v>
       </c>
       <c r="B67" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C67" s="1">
-        <v>0.50416666666666665</v>
+        <v>0.53194444444444444</v>
       </c>
       <c r="D67">
-        <v>1441</v>
+        <v>7138</v>
       </c>
       <c r="G67" s="1"/>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>34</v>
-      </c>
-      <c r="B68" t="s">
-        <v>35</v>
-      </c>
-      <c r="C68" s="1">
-        <v>0.50972222222222219</v>
-      </c>
-      <c r="D68">
-        <v>1910</v>
-      </c>
-      <c r="G68" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="C68" s="1"/>
+      <c r="E68">
+        <v>1468</v>
+      </c>
+      <c r="F68" t="s">
+        <v>22</v>
+      </c>
+      <c r="G68" s="1">
+        <v>0.55902777777777779</v>
+      </c>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>11</v>
+        <v>33</v>
       </c>
       <c r="C69" s="1"/>
       <c r="E69">
-        <v>319</v>
+        <v>1978</v>
       </c>
       <c r="F69" t="s">
-        <v>19</v>
+        <v>34</v>
       </c>
       <c r="G69" s="1">
-        <v>0.51388888888888884</v>
+        <v>0.56527777777777777</v>
       </c>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>42</v>
-      </c>
-      <c r="B70" t="s">
-        <v>43</v>
-      </c>
-      <c r="C70" s="1">
-        <v>0.52083333333333337</v>
-      </c>
-      <c r="D70">
-        <v>420</v>
-      </c>
-      <c r="G70" s="1"/>
+        <v>14</v>
+      </c>
+      <c r="C70" s="1"/>
+      <c r="E70">
+        <v>871</v>
+      </c>
+      <c r="F70" t="s">
+        <v>15</v>
+      </c>
+      <c r="G70" s="1">
+        <v>0.5708333333333333</v>
+      </c>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="C71" s="1"/>
       <c r="E71">
-        <v>1508</v>
+        <v>1032</v>
       </c>
       <c r="F71" t="s">
-        <v>27</v>
+        <v>41</v>
       </c>
       <c r="G71" s="1">
-        <v>0.52430555555555558</v>
+        <v>0.57291666666666663</v>
       </c>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="B72" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="C72" s="1">
-        <v>0.52500000000000002</v>
+        <v>0.59930555555555554</v>
       </c>
       <c r="D72">
-        <v>816</v>
+        <v>1290</v>
       </c>
       <c r="G72" s="1"/>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>44</v>
+        <v>35</v>
       </c>
       <c r="B73" t="s">
-        <v>45</v>
+        <v>30</v>
       </c>
       <c r="C73" s="1">
-        <v>0.52777777777777779</v>
+        <v>0.61388888888888882</v>
       </c>
       <c r="D73">
-        <v>1031</v>
+        <v>628</v>
       </c>
       <c r="G73" s="1"/>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="C74" s="1"/>
       <c r="E74">
-        <v>770</v>
+        <v>7139</v>
       </c>
       <c r="F74" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="G74" s="1">
-        <v>0.53125</v>
+        <v>0.6166666666666667</v>
       </c>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>42</v>
-      </c>
-      <c r="C75" s="1"/>
-      <c r="E75">
-        <v>421</v>
-      </c>
-      <c r="F75" t="s">
-        <v>43</v>
-      </c>
-      <c r="G75" s="1">
-        <v>0.54861111111111105</v>
-      </c>
+        <v>11</v>
+      </c>
+      <c r="B75" t="s">
+        <v>44</v>
+      </c>
+      <c r="C75" s="1">
+        <v>0.62152777777777779</v>
+      </c>
+      <c r="D75">
+        <v>651</v>
+      </c>
+      <c r="G75" s="1"/>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C76" s="1"/>
       <c r="E76">
-        <v>317</v>
+        <v>1130</v>
       </c>
       <c r="F76" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="G76" s="1">
-        <v>0.55555555555555558</v>
+        <v>0.64583333333333337</v>
       </c>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>7</v>
-      </c>
-      <c r="C77" s="1"/>
-      <c r="E77">
-        <v>1468</v>
-      </c>
-      <c r="F77" t="s">
-        <v>22</v>
-      </c>
-      <c r="G77" s="1">
-        <v>0.55902777777777779</v>
-      </c>
+        <v>11</v>
+      </c>
+      <c r="B77" t="s">
+        <v>27</v>
+      </c>
+      <c r="C77" s="1">
+        <v>0.66319444444444442</v>
+      </c>
+      <c r="D77">
+        <v>311</v>
+      </c>
+      <c r="G77" s="1"/>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>34</v>
-      </c>
-      <c r="C78" s="1"/>
-      <c r="E78">
-        <v>1978</v>
-      </c>
-      <c r="F78" t="s">
-        <v>35</v>
-      </c>
-      <c r="G78" s="1">
-        <v>0.56527777777777777</v>
-      </c>
+        <v>11</v>
+      </c>
+      <c r="B78" t="s">
+        <v>22</v>
+      </c>
+      <c r="C78" s="1">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="D78">
+        <v>367</v>
+      </c>
+      <c r="G78" s="1"/>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>14</v>
-      </c>
-      <c r="C79" s="1"/>
-      <c r="E79">
-        <v>871</v>
-      </c>
-      <c r="F79" t="s">
-        <v>15</v>
-      </c>
-      <c r="G79" s="1">
-        <v>0.5708333333333333</v>
-      </c>
+        <v>11</v>
+      </c>
+      <c r="B79" t="s">
+        <v>12</v>
+      </c>
+      <c r="C79" s="1">
+        <v>0.67013888888888884</v>
+      </c>
+      <c r="D79">
+        <v>370</v>
+      </c>
+      <c r="G79" s="1"/>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>44</v>
+        <v>35</v>
       </c>
       <c r="C80" s="1"/>
       <c r="E80">
-        <v>1032</v>
+        <v>629</v>
       </c>
       <c r="F80" t="s">
-        <v>45</v>
+        <v>30</v>
       </c>
       <c r="G80" s="1">
-        <v>0.57291666666666663</v>
+        <v>0.67013888888888884</v>
       </c>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="B81" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="C81" s="1">
-        <v>0.59930555555555554</v>
+        <v>0.67361111111111116</v>
       </c>
       <c r="D81">
-        <v>1290</v>
+        <v>441</v>
       </c>
       <c r="G81" s="1"/>
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>36</v>
+        <v>11</v>
       </c>
       <c r="B82" t="s">
-        <v>31</v>
+        <v>21</v>
       </c>
       <c r="C82" s="1">
-        <v>0.61388888888888882</v>
+        <v>0.68055555555555558</v>
       </c>
       <c r="D82">
-        <v>628</v>
+        <v>382</v>
       </c>
       <c r="G82" s="1"/>
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B83" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="C83" s="1">
-        <v>0.61875000000000002</v>
+        <v>0.68402777777777779</v>
       </c>
       <c r="D83">
-        <v>4317</v>
+        <v>318</v>
       </c>
       <c r="G83" s="1"/>
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>7</v>
-      </c>
-      <c r="C84" s="1"/>
-      <c r="E84">
-        <v>1130</v>
-      </c>
-      <c r="F84" t="s">
-        <v>22</v>
-      </c>
-      <c r="G84" s="1">
-        <v>0.64583333333333337</v>
-      </c>
+        <v>9</v>
+      </c>
+      <c r="B84" t="s">
+        <v>36</v>
+      </c>
+      <c r="C84" s="1">
+        <v>0.68888888888888899</v>
+      </c>
+      <c r="D84">
+        <v>4323</v>
+      </c>
+      <c r="G84" s="1"/>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>9</v>
-      </c>
-      <c r="C85" s="1"/>
-      <c r="E85">
-        <v>4322</v>
-      </c>
-      <c r="F85" t="s">
-        <v>37</v>
-      </c>
-      <c r="G85" s="1">
-        <v>0.66041666666666665</v>
-      </c>
+        <v>11</v>
+      </c>
+      <c r="B85" t="s">
+        <v>15</v>
+      </c>
+      <c r="C85" s="1">
+        <v>0.69097222222222221</v>
+      </c>
+      <c r="D85">
+        <v>322</v>
+      </c>
+      <c r="G85" s="1"/>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B86" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="C86" s="1">
-        <v>0.66319444444444442</v>
+        <v>0.69861111111111107</v>
       </c>
       <c r="D86">
-        <v>311</v>
+        <v>4321</v>
       </c>
       <c r="G86" s="1"/>
     </row>
@@ -1890,226 +1896,226 @@
       <c r="A87" t="s">
         <v>11</v>
       </c>
-      <c r="B87" t="s">
-        <v>22</v>
-      </c>
-      <c r="C87" s="1">
-        <v>0.66666666666666663</v>
-      </c>
-      <c r="D87">
-        <v>367</v>
-      </c>
-      <c r="G87" s="1"/>
+      <c r="C87" s="1"/>
+      <c r="E87">
+        <v>530</v>
+      </c>
+      <c r="F87" t="s">
+        <v>43</v>
+      </c>
+      <c r="G87" s="1">
+        <v>0.73263888888888884</v>
+      </c>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>11</v>
       </c>
-      <c r="B88" t="s">
-        <v>12</v>
-      </c>
-      <c r="C88" s="1">
-        <v>0.67013888888888884</v>
-      </c>
-      <c r="D88">
-        <v>370</v>
-      </c>
-      <c r="G88" s="1"/>
+      <c r="C88" s="1"/>
+      <c r="E88">
+        <v>617</v>
+      </c>
+      <c r="F88" t="s">
+        <v>19</v>
+      </c>
+      <c r="G88" s="1">
+        <v>0.73263888888888884</v>
+      </c>
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>36</v>
-      </c>
-      <c r="C89" s="1"/>
-      <c r="E89">
-        <v>629</v>
-      </c>
-      <c r="F89" t="s">
-        <v>31</v>
-      </c>
-      <c r="G89" s="1">
-        <v>0.67013888888888884</v>
-      </c>
+        <v>11</v>
+      </c>
+      <c r="B89" t="s">
+        <v>24</v>
+      </c>
+      <c r="C89" s="1">
+        <v>0.73611111111111116</v>
+      </c>
+      <c r="D89">
+        <v>397</v>
+      </c>
+      <c r="G89" s="1"/>
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>11</v>
       </c>
-      <c r="B90" t="s">
-        <v>28</v>
-      </c>
-      <c r="C90" s="1">
-        <v>0.67361111111111116</v>
-      </c>
-      <c r="D90">
-        <v>441</v>
-      </c>
-      <c r="G90" s="1"/>
+      <c r="C90" s="1"/>
+      <c r="E90">
+        <v>560</v>
+      </c>
+      <c r="F90" t="s">
+        <v>25</v>
+      </c>
+      <c r="G90" s="1">
+        <v>0.73611111111111116</v>
+      </c>
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>11</v>
       </c>
-      <c r="B91" t="s">
-        <v>21</v>
-      </c>
-      <c r="C91" s="1">
-        <v>0.68055555555555558</v>
-      </c>
-      <c r="D91">
-        <v>382</v>
-      </c>
-      <c r="G91" s="1"/>
+      <c r="C91" s="1"/>
+      <c r="E91">
+        <v>534</v>
+      </c>
+      <c r="F91" t="s">
+        <v>18</v>
+      </c>
+      <c r="G91" s="1">
+        <v>0.73958333333333337</v>
+      </c>
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>11</v>
       </c>
-      <c r="B92" t="s">
-        <v>19</v>
-      </c>
-      <c r="C92" s="1">
-        <v>0.68402777777777779</v>
-      </c>
-      <c r="D92">
-        <v>318</v>
-      </c>
-      <c r="G92" s="1"/>
+      <c r="C92" s="1"/>
+      <c r="E92">
+        <v>588</v>
+      </c>
+      <c r="F92" t="s">
+        <v>23</v>
+      </c>
+      <c r="G92" s="1">
+        <v>0.73958333333333337</v>
+      </c>
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>9</v>
       </c>
-      <c r="B93" t="s">
-        <v>37</v>
-      </c>
-      <c r="C93" s="1">
-        <v>0.68888888888888899</v>
-      </c>
-      <c r="D93">
-        <v>4323</v>
-      </c>
-      <c r="G93" s="1"/>
+      <c r="C93" s="1"/>
+      <c r="E93">
+        <v>4308</v>
+      </c>
+      <c r="F93" t="s">
+        <v>8</v>
+      </c>
+      <c r="G93" s="1">
+        <v>0.73958333333333337</v>
+      </c>
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>11</v>
       </c>
-      <c r="B94" t="s">
-        <v>15</v>
-      </c>
-      <c r="C94" s="1">
-        <v>0.69097222222222221</v>
-      </c>
-      <c r="D94">
-        <v>322</v>
-      </c>
-      <c r="G94" s="1"/>
+      <c r="C94" s="1"/>
+      <c r="E94">
+        <v>448</v>
+      </c>
+      <c r="F94" t="s">
+        <v>20</v>
+      </c>
+      <c r="G94" s="1">
+        <v>0.74305555555555558</v>
+      </c>
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>11</v>
+        <v>37</v>
       </c>
       <c r="B95" t="s">
         <v>23</v>
       </c>
       <c r="C95" s="1">
-        <v>0.69097222222222221</v>
+        <v>0.75</v>
       </c>
       <c r="D95">
-        <v>555</v>
+        <v>222</v>
       </c>
       <c r="G95" s="1"/>
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>9</v>
+        <v>46</v>
       </c>
       <c r="B96" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="C96" s="1">
-        <v>0.69791666666666663</v>
+        <v>0.7631944444444444</v>
       </c>
       <c r="D96">
-        <v>4327</v>
+        <v>4040</v>
       </c>
       <c r="G96" s="1"/>
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>11</v>
-      </c>
-      <c r="C97" s="1"/>
-      <c r="E97">
-        <v>617</v>
-      </c>
-      <c r="F97" t="s">
-        <v>19</v>
-      </c>
-      <c r="G97" s="1">
-        <v>0.73263888888888884</v>
-      </c>
+        <v>17</v>
+      </c>
+      <c r="B97" t="s">
+        <v>47</v>
+      </c>
+      <c r="C97" s="1">
+        <v>0.77083333333333337</v>
+      </c>
+      <c r="D97">
+        <v>931</v>
+      </c>
+      <c r="G97" s="1"/>
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>9</v>
       </c>
-      <c r="B98" t="s">
-        <v>19</v>
-      </c>
-      <c r="C98" s="1">
-        <v>0.73333333333333328</v>
-      </c>
-      <c r="D98">
-        <v>4351</v>
-      </c>
-      <c r="G98" s="1"/>
+      <c r="C98" s="1"/>
+      <c r="E98">
+        <v>4312</v>
+      </c>
+      <c r="F98" t="s">
+        <v>10</v>
+      </c>
+      <c r="G98" s="1">
+        <v>0.77569444444444446</v>
+      </c>
     </row>
     <row r="99" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>11</v>
       </c>
-      <c r="B99" t="s">
-        <v>24</v>
-      </c>
-      <c r="C99" s="1">
-        <v>0.73611111111111116</v>
-      </c>
-      <c r="D99">
-        <v>397</v>
-      </c>
-      <c r="G99" s="1"/>
+      <c r="C99" s="1"/>
+      <c r="E99">
+        <v>528</v>
+      </c>
+      <c r="F99" t="s">
+        <v>8</v>
+      </c>
+      <c r="G99" s="1">
+        <v>0.77777777777777779</v>
+      </c>
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>11</v>
       </c>
-      <c r="C100" s="1"/>
-      <c r="E100">
-        <v>560</v>
-      </c>
-      <c r="F100" t="s">
-        <v>25</v>
-      </c>
-      <c r="G100" s="1">
-        <v>0.73611111111111116</v>
-      </c>
+      <c r="B100" t="s">
+        <v>30</v>
+      </c>
+      <c r="C100" s="1">
+        <v>0.79513888888888884</v>
+      </c>
+      <c r="D100">
+        <v>431</v>
+      </c>
+      <c r="G100" s="1"/>
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>11</v>
       </c>
-      <c r="C101" s="1"/>
-      <c r="E101">
-        <v>620</v>
-      </c>
-      <c r="F101" t="s">
-        <v>8</v>
-      </c>
-      <c r="G101" s="1">
-        <v>0.73611111111111116</v>
-      </c>
+      <c r="B101" t="s">
+        <v>10</v>
+      </c>
+      <c r="C101" s="1">
+        <v>0.8125</v>
+      </c>
+      <c r="D101">
+        <v>583</v>
+      </c>
+      <c r="G101" s="1"/>
     </row>
     <row r="102" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
@@ -2117,28 +2123,28 @@
       </c>
       <c r="C102" s="1"/>
       <c r="E102">
-        <v>534</v>
+        <v>570</v>
       </c>
       <c r="F102" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="G102" s="1">
-        <v>0.73958333333333337</v>
+        <v>0.8125</v>
       </c>
     </row>
     <row r="103" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>11</v>
+        <v>37</v>
       </c>
       <c r="C103" s="1"/>
       <c r="E103">
-        <v>588</v>
+        <v>222</v>
       </c>
       <c r="F103" t="s">
-        <v>23</v>
+        <v>38</v>
       </c>
       <c r="G103" s="1">
-        <v>0.73958333333333337</v>
+        <v>0.8125</v>
       </c>
     </row>
     <row r="104" spans="1:7" x14ac:dyDescent="0.25">
@@ -2147,102 +2153,102 @@
       </c>
       <c r="C104" s="1"/>
       <c r="E104">
-        <v>4308</v>
+        <v>4300</v>
       </c>
       <c r="F104" t="s">
-        <v>8</v>
+        <v>30</v>
       </c>
       <c r="G104" s="1">
-        <v>0.73958333333333337</v>
+        <v>0.81597222222222221</v>
       </c>
     </row>
     <row r="105" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="C105" s="1"/>
       <c r="E105">
-        <v>448</v>
+        <v>932</v>
       </c>
       <c r="F105" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="G105" s="1">
-        <v>0.74305555555555558</v>
+        <v>0.81597222222222221</v>
       </c>
     </row>
     <row r="106" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>38</v>
+        <v>11</v>
       </c>
       <c r="B106" t="s">
-        <v>23</v>
+        <v>8</v>
       </c>
       <c r="C106" s="1">
-        <v>0.75</v>
+        <v>0.82638888888888884</v>
       </c>
       <c r="D106">
-        <v>222</v>
+        <v>523</v>
       </c>
       <c r="G106" s="1"/>
     </row>
     <row r="107" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>9</v>
-      </c>
-      <c r="C107" s="1"/>
-      <c r="E107">
-        <v>4312</v>
-      </c>
-      <c r="F107" t="s">
-        <v>10</v>
-      </c>
-      <c r="G107" s="1">
-        <v>0.77569444444444446</v>
-      </c>
+        <v>11</v>
+      </c>
+      <c r="B107" t="s">
+        <v>29</v>
+      </c>
+      <c r="C107" s="1">
+        <v>0.84375</v>
+      </c>
+      <c r="D107">
+        <v>627</v>
+      </c>
+      <c r="G107" s="1"/>
     </row>
     <row r="108" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>11</v>
-      </c>
-      <c r="C108" s="1"/>
-      <c r="E108">
-        <v>528</v>
-      </c>
-      <c r="F108" t="s">
-        <v>8</v>
-      </c>
-      <c r="G108" s="1">
-        <v>0.77777777777777779</v>
-      </c>
+        <v>7</v>
+      </c>
+      <c r="B108" t="s">
+        <v>22</v>
+      </c>
+      <c r="C108" s="1">
+        <v>0.84513888888888899</v>
+      </c>
+      <c r="D108">
+        <v>1461</v>
+      </c>
+      <c r="G108" s="1"/>
     </row>
     <row r="109" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>11</v>
-      </c>
-      <c r="C109" s="1"/>
-      <c r="E109">
-        <v>566</v>
-      </c>
-      <c r="F109" t="s">
-        <v>26</v>
-      </c>
-      <c r="G109" s="1">
-        <v>0.78819444444444442</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="B109" t="s">
+        <v>15</v>
+      </c>
+      <c r="C109" s="1">
+        <v>0.84861111111111109</v>
+      </c>
+      <c r="D109">
+        <v>881</v>
+      </c>
+      <c r="G109" s="1"/>
     </row>
     <row r="110" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>11</v>
       </c>
       <c r="B110" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="C110" s="1">
-        <v>0.79513888888888884</v>
+        <v>0.85069444444444442</v>
       </c>
       <c r="D110">
-        <v>431</v>
+        <v>449</v>
       </c>
       <c r="G110" s="1"/>
     </row>
@@ -2250,59 +2256,59 @@
       <c r="A111" t="s">
         <v>11</v>
       </c>
-      <c r="B111" t="s">
+      <c r="C111" s="1"/>
+      <c r="E111">
+        <v>590</v>
+      </c>
+      <c r="F111" t="s">
         <v>10</v>
       </c>
-      <c r="C111" s="1">
-        <v>0.8125</v>
-      </c>
-      <c r="D111">
-        <v>583</v>
-      </c>
-      <c r="G111" s="1"/>
+      <c r="G111" s="1">
+        <v>0.85416666666666663</v>
+      </c>
     </row>
     <row r="112" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>11</v>
       </c>
-      <c r="C112" s="1"/>
-      <c r="E112">
-        <v>570</v>
-      </c>
-      <c r="F112" t="s">
-        <v>26</v>
-      </c>
-      <c r="G112" s="1">
-        <v>0.8125</v>
-      </c>
+      <c r="B112" t="s">
+        <v>28</v>
+      </c>
+      <c r="C112" s="1">
+        <v>0.86111111111111116</v>
+      </c>
+      <c r="D112">
+        <v>443</v>
+      </c>
+      <c r="G112" s="1"/>
     </row>
     <row r="113" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>38</v>
-      </c>
-      <c r="C113" s="1"/>
-      <c r="E113">
-        <v>222</v>
-      </c>
-      <c r="F113" t="s">
-        <v>39</v>
-      </c>
-      <c r="G113" s="1">
-        <v>0.8125</v>
-      </c>
+        <v>11</v>
+      </c>
+      <c r="B113" t="s">
+        <v>25</v>
+      </c>
+      <c r="C113" s="1">
+        <v>0.86805555555555558</v>
+      </c>
+      <c r="D113">
+        <v>563</v>
+      </c>
+      <c r="G113" s="1"/>
     </row>
     <row r="114" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>11</v>
       </c>
       <c r="B114" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C114" s="1">
-        <v>0.81597222222222221</v>
+        <v>0.875</v>
       </c>
       <c r="D114">
-        <v>425</v>
+        <v>535</v>
       </c>
       <c r="G114" s="1"/>
     </row>
@@ -2311,13 +2317,13 @@
         <v>11</v>
       </c>
       <c r="B115" t="s">
-        <v>8</v>
+        <v>23</v>
       </c>
       <c r="C115" s="1">
-        <v>0.82638888888888884</v>
+        <v>0.87847222222222221</v>
       </c>
       <c r="D115">
-        <v>523</v>
+        <v>589</v>
       </c>
       <c r="G115" s="1"/>
     </row>
@@ -2326,13 +2332,13 @@
         <v>11</v>
       </c>
       <c r="B116" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="C116" s="1">
-        <v>0.83680555555555558</v>
+        <v>0.87847222222222221</v>
       </c>
       <c r="D116">
-        <v>393</v>
+        <v>616</v>
       </c>
       <c r="G116" s="1"/>
     </row>
@@ -2341,13 +2347,13 @@
         <v>11</v>
       </c>
       <c r="B117" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="C117" s="1">
-        <v>0.84375</v>
+        <v>0.88888888888888884</v>
       </c>
       <c r="D117">
-        <v>445</v>
+        <v>608</v>
       </c>
       <c r="G117" s="1"/>
     </row>
@@ -2356,60 +2362,60 @@
         <v>11</v>
       </c>
       <c r="B118" t="s">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="C118" s="1">
-        <v>0.84375</v>
+        <v>0.90972222222222221</v>
       </c>
       <c r="D118">
-        <v>627</v>
+        <v>585</v>
       </c>
       <c r="G118" s="1"/>
     </row>
     <row r="119" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>7</v>
-      </c>
-      <c r="B119" t="s">
-        <v>22</v>
-      </c>
-      <c r="C119" s="1">
-        <v>0.84513888888888899</v>
-      </c>
-      <c r="D119">
-        <v>1461</v>
-      </c>
-      <c r="G119" s="1"/>
+        <v>11</v>
+      </c>
+      <c r="C119" s="1"/>
+      <c r="E119">
+        <v>365</v>
+      </c>
+      <c r="F119" t="s">
+        <v>21</v>
+      </c>
+      <c r="G119" s="1">
+        <v>0.92013888888888884</v>
+      </c>
     </row>
     <row r="120" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>14</v>
-      </c>
-      <c r="B120" t="s">
-        <v>15</v>
-      </c>
-      <c r="C120" s="1">
-        <v>0.84861111111111109</v>
-      </c>
-      <c r="D120">
-        <v>881</v>
-      </c>
-      <c r="G120" s="1"/>
+        <v>11</v>
+      </c>
+      <c r="C120" s="1"/>
+      <c r="E120">
+        <v>580</v>
+      </c>
+      <c r="F120" t="s">
+        <v>10</v>
+      </c>
+      <c r="G120" s="1">
+        <v>0.92013888888888884</v>
+      </c>
     </row>
     <row r="121" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>11</v>
       </c>
-      <c r="B121" t="s">
-        <v>20</v>
-      </c>
-      <c r="C121" s="1">
-        <v>0.85069444444444442</v>
-      </c>
-      <c r="D121">
-        <v>449</v>
-      </c>
-      <c r="G121" s="1"/>
+      <c r="C121" s="1"/>
+      <c r="E121">
+        <v>429</v>
+      </c>
+      <c r="F121" t="s">
+        <v>16</v>
+      </c>
+      <c r="G121" s="1">
+        <v>0.92361111111111116</v>
+      </c>
     </row>
     <row r="122" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
@@ -2417,283 +2423,161 @@
       </c>
       <c r="C122" s="1"/>
       <c r="E122">
-        <v>690</v>
+        <v>457</v>
       </c>
       <c r="F122" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="G122" s="1">
-        <v>0.85416666666666663</v>
+        <v>0.92361111111111116</v>
       </c>
     </row>
     <row r="123" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>11</v>
       </c>
-      <c r="B123" t="s">
-        <v>25</v>
-      </c>
-      <c r="C123" s="1">
-        <v>0.86805555555555558</v>
-      </c>
-      <c r="D123">
-        <v>563</v>
-      </c>
-      <c r="G123" s="1"/>
+      <c r="C123" s="1"/>
+      <c r="E123">
+        <v>593</v>
+      </c>
+      <c r="F123" t="s">
+        <v>42</v>
+      </c>
+      <c r="G123" s="1">
+        <v>0.92361111111111116</v>
+      </c>
     </row>
     <row r="124" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>9</v>
-      </c>
-      <c r="B124" t="s">
-        <v>27</v>
-      </c>
-      <c r="C124" s="1">
-        <v>0.86944444444444446</v>
-      </c>
-      <c r="D124">
-        <v>4339</v>
-      </c>
-      <c r="G124" s="1"/>
+        <v>11</v>
+      </c>
+      <c r="C124" s="1"/>
+      <c r="E124">
+        <v>578</v>
+      </c>
+      <c r="F124" t="s">
+        <v>23</v>
+      </c>
+      <c r="G124" s="1">
+        <v>0.93055555555555558</v>
+      </c>
     </row>
     <row r="125" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>11</v>
       </c>
-      <c r="B125" t="s">
-        <v>18</v>
-      </c>
-      <c r="C125" s="1">
-        <v>0.875</v>
-      </c>
-      <c r="D125">
-        <v>535</v>
-      </c>
-      <c r="G125" s="1"/>
+      <c r="C125" s="1"/>
+      <c r="E125">
+        <v>651</v>
+      </c>
+      <c r="F125" t="s">
+        <v>19</v>
+      </c>
+      <c r="G125" s="1">
+        <v>0.93402777777777779</v>
+      </c>
     </row>
     <row r="126" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>11</v>
       </c>
-      <c r="B126" t="s">
-        <v>15</v>
-      </c>
-      <c r="C126" s="1">
-        <v>0.87847222222222221</v>
-      </c>
-      <c r="D126">
-        <v>316</v>
-      </c>
-      <c r="G126" s="1"/>
+      <c r="C126" s="1"/>
+      <c r="E126">
+        <v>574</v>
+      </c>
+      <c r="F126" t="s">
+        <v>18</v>
+      </c>
+      <c r="G126" s="1">
+        <v>0.9375</v>
+      </c>
     </row>
     <row r="127" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>11</v>
       </c>
-      <c r="B127" t="s">
-        <v>23</v>
-      </c>
-      <c r="C127" s="1">
-        <v>0.87847222222222221</v>
-      </c>
-      <c r="D127">
-        <v>557</v>
-      </c>
-      <c r="G127" s="1"/>
+      <c r="C127" s="1"/>
+      <c r="E127">
+        <v>315</v>
+      </c>
+      <c r="F127" t="s">
+        <v>24</v>
+      </c>
+      <c r="G127" s="1">
+        <v>0.94097222222222221</v>
+      </c>
     </row>
     <row r="128" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>11</v>
       </c>
-      <c r="B128" t="s">
-        <v>23</v>
-      </c>
-      <c r="C128" s="1">
-        <v>0.87847222222222221</v>
-      </c>
-      <c r="D128">
-        <v>589</v>
-      </c>
-      <c r="G128" s="1"/>
+      <c r="C128" s="1"/>
+      <c r="E128">
+        <v>568</v>
+      </c>
+      <c r="F128" t="s">
+        <v>26</v>
+      </c>
+      <c r="G128" s="1">
+        <v>0.95486111111111116</v>
+      </c>
     </row>
     <row r="129" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B129" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C129" s="1">
-        <v>0.87847222222222221</v>
+        <v>0.98263888888888884</v>
       </c>
       <c r="D129">
-        <v>616</v>
-      </c>
-      <c r="G129" s="1"/>
+        <v>878</v>
+      </c>
     </row>
     <row r="130" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A130" t="s">
-        <v>11</v>
-      </c>
       <c r="C130" s="1"/>
-      <c r="E130">
-        <v>365</v>
-      </c>
-      <c r="F130" t="s">
-        <v>21</v>
-      </c>
-      <c r="G130" s="1">
-        <v>0.92013888888888884</v>
-      </c>
+      <c r="G130" s="1"/>
     </row>
     <row r="131" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A131" t="s">
-        <v>11</v>
-      </c>
       <c r="C131" s="1"/>
-      <c r="E131">
-        <v>580</v>
-      </c>
-      <c r="F131" t="s">
-        <v>10</v>
-      </c>
-      <c r="G131" s="1">
-        <v>0.92013888888888884</v>
-      </c>
+      <c r="G131" s="1"/>
     </row>
     <row r="132" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A132" t="s">
-        <v>11</v>
-      </c>
       <c r="C132" s="1"/>
-      <c r="E132">
-        <v>429</v>
-      </c>
-      <c r="F132" t="s">
-        <v>16</v>
-      </c>
-      <c r="G132" s="1">
-        <v>0.92361111111111116</v>
-      </c>
+      <c r="G132" s="1"/>
     </row>
     <row r="133" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A133" t="s">
-        <v>11</v>
-      </c>
       <c r="C133" s="1"/>
-      <c r="E133">
-        <v>457</v>
-      </c>
-      <c r="F133" t="s">
-        <v>13</v>
-      </c>
-      <c r="G133" s="1">
-        <v>0.92361111111111116</v>
-      </c>
+      <c r="G133" s="1"/>
     </row>
     <row r="134" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A134" t="s">
-        <v>11</v>
-      </c>
       <c r="C134" s="1"/>
-      <c r="E134">
-        <v>578</v>
-      </c>
-      <c r="F134" t="s">
-        <v>23</v>
-      </c>
-      <c r="G134" s="1">
-        <v>0.93055555555555558</v>
-      </c>
+      <c r="G134" s="1"/>
     </row>
     <row r="135" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A135" t="s">
-        <v>11</v>
-      </c>
       <c r="C135" s="1"/>
-      <c r="E135">
-        <v>627</v>
-      </c>
-      <c r="F135" t="s">
-        <v>19</v>
-      </c>
-      <c r="G135" s="1">
-        <v>0.93402777777777779</v>
-      </c>
+      <c r="G135" s="1"/>
     </row>
     <row r="136" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A136" t="s">
-        <v>11</v>
-      </c>
       <c r="C136" s="1"/>
-      <c r="E136">
-        <v>574</v>
-      </c>
-      <c r="F136" t="s">
-        <v>18</v>
-      </c>
-      <c r="G136" s="1">
-        <v>0.9375</v>
-      </c>
+      <c r="G136" s="1"/>
     </row>
     <row r="137" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A137" t="s">
-        <v>11</v>
-      </c>
       <c r="C137" s="1"/>
-      <c r="E137">
-        <v>315</v>
-      </c>
-      <c r="F137" t="s">
-        <v>24</v>
-      </c>
-      <c r="G137" s="1">
-        <v>0.94097222222222221</v>
-      </c>
+      <c r="G137" s="1"/>
     </row>
     <row r="138" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A138" t="s">
-        <v>11</v>
-      </c>
       <c r="C138" s="1"/>
-      <c r="E138">
-        <v>452</v>
-      </c>
-      <c r="F138" t="s">
-        <v>20</v>
-      </c>
-      <c r="G138" s="1">
-        <v>0.95138888888888884</v>
-      </c>
+      <c r="G138" s="1"/>
     </row>
     <row r="139" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A139" t="s">
-        <v>11</v>
-      </c>
       <c r="C139" s="1"/>
-      <c r="E139">
-        <v>568</v>
-      </c>
-      <c r="F139" t="s">
-        <v>26</v>
-      </c>
-      <c r="G139" s="1">
-        <v>0.95486111111111116</v>
-      </c>
+      <c r="G139" s="1"/>
     </row>
     <row r="140" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A140" t="s">
-        <v>14</v>
-      </c>
-      <c r="B140" t="s">
-        <v>15</v>
-      </c>
-      <c r="C140" s="1">
-        <v>0.98263888888888884</v>
-      </c>
-      <c r="D140">
-        <v>878</v>
-      </c>
+      <c r="C140" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>